<commit_message>
Clean UNIPA (minus 3 transcriptions)
</commit_message>
<xml_diff>
--- a/input_xlsx/Flora 002.xlsx
+++ b/input_xlsx/Flora 002.xlsx
@@ -2465,7 +2465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="113">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -2632,9 +2632,6 @@
     <t>PULAU ROON</t>
   </si>
   <si>
-    <t>DESA YENDE</t>
-  </si>
-  <si>
     <t>TIDAK DISEBUTKAN JUMLAH INDIVIDU DARI KE 11 JENIS YANG TERDAPAT DI PULAU ROON DESA YENDE</t>
   </si>
   <si>
@@ -2644,27 +2641,9 @@
     <t>134.540585</t>
   </si>
   <si>
-    <t>DESA MENARBU</t>
-  </si>
-  <si>
-    <t>TIDAK DISEBUTKAN JUMLAH INDIVIDU DARI KE 11 JENIS YANG TERDAPAT DI PULAU ROON DESA MENARBU</t>
-  </si>
-  <si>
-    <t>134.5596089</t>
-  </si>
-  <si>
-    <t>-2.3875472</t>
-  </si>
-  <si>
     <t>2005-04-1/2005-04-30</t>
   </si>
   <si>
-    <t>DESA KAYOP</t>
-  </si>
-  <si>
-    <t>TIDAK DISEBUTKAN JUMLAH INDIVIDU DARI KE 11 JENIS YANG TERDAPAT DI PULAU ROON DESA KAYOP</t>
-  </si>
-  <si>
     <t>HUMAN OBSERVATION</t>
   </si>
   <si>
@@ -2674,12 +2653,6 @@
     <t>PR001-dy001</t>
   </si>
   <si>
-    <t>PR002-Dm001</t>
-  </si>
-  <si>
-    <t>PR003-DK001</t>
-  </si>
-  <si>
     <t>Areca catechu L</t>
   </si>
   <si>
@@ -2788,59 +2761,56 @@
     <t>Ptychosperma sp tidak disebutkan jumlahnya</t>
   </si>
   <si>
+    <t>DESA YENDE, DESA MENARBU, DESA KAYOP</t>
+  </si>
+  <si>
     <t>UNIPA-2006ES-AF002</t>
   </si>
   <si>
     <t>UNIPA-2006ES-AF002-PR001</t>
   </si>
   <si>
-    <t>UNIPA-2006ES-AF002-PR002</t>
-  </si>
-  <si>
-    <t>UNIPA-2006ES-AF002-PR003</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE001</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE002</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE003</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE004</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE005</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE006</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE007</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE008</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE009</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE010</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-VE011</t>
-  </si>
-  <si>
-    <t>uNIPA -2006ES-AF002-PR002-VE001</t>
+    <t>UNIPA -2006ES-AF002-PR001-EM001</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM002</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM003</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM004</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM005</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM006</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM007</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM008</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM009</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM010</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM011</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-EM012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3117,7 +3087,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
@@ -3141,9 +3111,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3575,17 +3542,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1048576"/>
+      <selection pane="bottomLeft" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.25" customWidth="1"/>
+    <col min="2" max="2" width="27.08203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.5" style="8" bestFit="1" customWidth="1"/>
@@ -3603,7 +3570,7 @@
     <col min="20" max="20" width="90.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -3665,15 +3632,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -3688,7 +3655,7 @@
         <v>48</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>52</v>
@@ -3715,173 +3682,61 @@
         <v>54</v>
       </c>
       <c r="S2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" t="s">
         <v>55</v>
       </c>
-      <c r="T2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" t="s">
-        <v>54</v>
-      </c>
-      <c r="S3" t="s">
-        <v>59</v>
-      </c>
-      <c r="T3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" t="s">
-        <v>49</v>
-      </c>
-      <c r="P4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R4" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" t="s">
-        <v>64</v>
-      </c>
-      <c r="T4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:20">
+      <c r="E3"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="E4"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="1:20">
       <c r="E5"/>
       <c r="K5" s="12"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20">
       <c r="E6"/>
       <c r="K6" s="12"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20">
       <c r="E7"/>
       <c r="K7" s="12"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20">
       <c r="E8"/>
       <c r="K8" s="12"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20">
       <c r="E9"/>
       <c r="K9" s="12"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20">
       <c r="E10"/>
       <c r="K10" s="12"/>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20">
       <c r="E11"/>
       <c r="K11" s="12"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20">
       <c r="E12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E13"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="E14"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -3907,7 +3762,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
@@ -3928,7 +3783,7 @@
     <col min="17" max="17" width="83.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -3981,30 +3836,30 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>52</v>
@@ -4019,36 +3874,36 @@
         <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>52</v>
@@ -4063,36 +3918,36 @@
         <v>44</v>
       </c>
       <c r="P3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
         <v>63</v>
       </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>52</v>
@@ -4107,36 +3962,36 @@
         <v>44</v>
       </c>
       <c r="P4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>52</v>
@@ -4151,36 +4006,36 @@
         <v>44</v>
       </c>
       <c r="P5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>52</v>
@@ -4195,36 +4050,36 @@
         <v>44</v>
       </c>
       <c r="P6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>72</v>
-      </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>52</v>
@@ -4239,36 +4094,36 @@
         <v>44</v>
       </c>
       <c r="P7" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>52</v>
@@ -4283,36 +4138,36 @@
         <v>44</v>
       </c>
       <c r="P8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
         <v>108</v>
       </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="E9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" t="s">
-        <v>72</v>
-      </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>52</v>
@@ -4327,36 +4182,36 @@
         <v>44</v>
       </c>
       <c r="P9" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" t="s">
-        <v>72</v>
-      </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>52</v>
@@ -4371,36 +4226,36 @@
         <v>44</v>
       </c>
       <c r="P10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>108</v>
-      </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>52</v>
@@ -4415,36 +4270,36 @@
         <v>44</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>52</v>
@@ -4459,42 +4314,42 @@
         <v>44</v>
       </c>
       <c r="P12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
+      <c r="H13" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" t="s">
-        <v>76</v>
-      </c>
       <c r="I13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="K13" t="s">
         <v>45</v>
@@ -4503,203 +4358,203 @@
         <v>44</v>
       </c>
       <c r="P13" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="F14" s="9"/>
       <c r="I14" s="12"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17">
       <c r="F15" s="9"/>
       <c r="I15" s="12"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17">
       <c r="F16" s="9"/>
       <c r="I16" s="12"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:10">
       <c r="F17" s="9"/>
       <c r="I17" s="12"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:10">
       <c r="F18" s="9"/>
       <c r="I18" s="12"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:10">
       <c r="F19" s="9"/>
       <c r="I19" s="12"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:10">
       <c r="F20" s="9"/>
       <c r="I20" s="12"/>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:10">
       <c r="F21" s="9"/>
       <c r="I21" s="12"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:10">
       <c r="F22" s="9"/>
       <c r="I22" s="12"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:10">
       <c r="F23" s="9"/>
       <c r="I23" s="12"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:10">
       <c r="F24" s="9"/>
       <c r="I24" s="12"/>
       <c r="J24" s="11"/>
     </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="6:10">
       <c r="F25" s="9"/>
       <c r="I25" s="12"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:10">
       <c r="F26" s="9"/>
       <c r="I26" s="12"/>
       <c r="J26" s="11"/>
     </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:10">
       <c r="F27" s="9"/>
       <c r="I27" s="12"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="6:10">
       <c r="F28" s="9"/>
       <c r="I28" s="12"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="6:10">
       <c r="F29" s="9"/>
       <c r="I29" s="12"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="6:10">
       <c r="F30" s="9"/>
       <c r="I30" s="12"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="6:10">
       <c r="F31" s="9"/>
       <c r="I31" s="12"/>
       <c r="J31" s="11"/>
     </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="6:10">
       <c r="F32" s="9"/>
       <c r="I32" s="12"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:10">
       <c r="F33" s="9"/>
       <c r="I33" s="12"/>
       <c r="J33" s="11"/>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:10">
       <c r="F34" s="9"/>
       <c r="I34" s="12"/>
       <c r="J34" s="11"/>
     </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:10">
       <c r="F35" s="9"/>
       <c r="I35" s="12"/>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="6:10">
       <c r="I36" s="12"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="6:10">
       <c r="I37" s="12"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="6:10">
       <c r="I38" s="12"/>
       <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="6:10">
       <c r="I39" s="12"/>
       <c r="J39" s="11"/>
     </row>
-    <row r="40" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="6:10">
       <c r="I40" s="12"/>
       <c r="J40" s="11"/>
     </row>
-    <row r="41" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="6:10">
       <c r="I41" s="12"/>
       <c r="J41" s="11"/>
     </row>
-    <row r="42" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="6:10">
       <c r="I42" s="12"/>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="6:10">
       <c r="I43" s="12"/>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="6:10">
       <c r="I44" s="12"/>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="6:10">
       <c r="I45" s="12"/>
       <c r="J45" s="11"/>
     </row>
-    <row r="46" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="6:10">
       <c r="I46" s="12"/>
       <c r="J46" s="11"/>
     </row>
-    <row r="47" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="6:10">
       <c r="I47" s="12"/>
       <c r="J47" s="11"/>
     </row>
-    <row r="48" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="6:10">
       <c r="I48" s="12"/>
       <c r="J48" s="11"/>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:10">
       <c r="I49" s="12"/>
       <c r="J49" s="11"/>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:10">
       <c r="I50" s="12"/>
       <c r="J50" s="11"/>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:10">
       <c r="I51" s="12"/>
       <c r="J51" s="11"/>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:10">
       <c r="I52" s="12"/>
       <c r="J52" s="11"/>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="9:10">
       <c r="I53" s="12"/>
       <c r="J53" s="11"/>
     </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="9:10">
       <c r="I54" s="12"/>
       <c r="J54" s="11"/>
     </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:10">
       <c r="I55" s="12"/>
       <c r="J55" s="11"/>
     </row>
-    <row r="56" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="9:10">
       <c r="I56" s="12"/>
       <c r="J56" s="11"/>
     </row>
@@ -4725,7 +4580,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
@@ -4739,7 +4594,7 @@
     <col min="10" max="10" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -4771,7 +4626,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="J2" s="8"/>
     </row>
   </sheetData>
@@ -4789,7 +4644,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
@@ -4802,7 +4657,7 @@
     <col min="9" max="9" width="22.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Clean unipa minor data
</commit_message>
<xml_diff>
--- a/input_xlsx/Flora 002.xlsx
+++ b/input_xlsx/Flora 002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20620" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -2761,49 +2761,49 @@
     <t>Ptychosperma sp tidak disebutkan jumlahnya</t>
   </si>
   <si>
+    <t>UNIPA-2006ES-AF002</t>
+  </si>
+  <si>
+    <t>UNIPA-2006ES-AF002-PR001</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE001</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE002</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE003</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE004</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE005</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE006</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE007</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE008</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE009</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE010</t>
+  </si>
+  <si>
+    <t>UNIPA -2006ES-AF002-PR001-VE011</t>
+  </si>
+  <si>
+    <t>uNIPA -2006ES-AF002-PR002-VE001</t>
+  </si>
+  <si>
     <t>DESA YENDE, DESA MENARBU, DESA KAYOP</t>
-  </si>
-  <si>
-    <t>UNIPA-2006ES-AF002</t>
-  </si>
-  <si>
-    <t>UNIPA-2006ES-AF002-PR001</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM001</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM002</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM003</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM004</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM005</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM006</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM007</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM008</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM009</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM010</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM011</t>
-  </si>
-  <si>
-    <t>UNIPA -2006ES-AF002-PR001-EM012</t>
   </si>
 </sst>
 </file>
@@ -3087,7 +3087,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
@@ -3111,6 +3111,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3542,17 +3545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B2"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.08203125" customWidth="1"/>
+    <col min="2" max="2" width="26.25" customWidth="1"/>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.5" style="8" bestFit="1" customWidth="1"/>
@@ -3566,7 +3569,7 @@
     <col min="14" max="16" width="13.5" customWidth="1"/>
     <col min="17" max="17" width="18.75" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.25" customWidth="1"/>
-    <col min="19" max="19" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40" customWidth="1"/>
     <col min="20" max="20" width="90.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3634,10 +3637,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -3682,7 +3685,7 @@
         <v>54</v>
       </c>
       <c r="S2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="T2" t="s">
         <v>55</v>
@@ -3690,13 +3693,13 @@
     </row>
     <row r="3" spans="1:20">
       <c r="E3"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:20">
       <c r="E4"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="11"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:20">
       <c r="E5"/>
@@ -3737,6 +3740,16 @@
       <c r="E12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="E13"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="E14"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
@@ -3758,7 +3771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -3838,10 +3851,10 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -3882,10 +3895,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
         <v>59</v>
@@ -3926,10 +3939,10 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
@@ -3970,10 +3983,10 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -4014,10 +4027,10 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
@@ -4058,10 +4071,10 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -4102,10 +4115,10 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -4146,10 +4159,10 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
@@ -4190,10 +4203,10 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
@@ -4234,10 +4247,10 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>59</v>
@@ -4278,10 +4291,10 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>59</v>
@@ -4322,10 +4335,10 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Add andika + UNIPA transcription revisions
</commit_message>
<xml_diff>
--- a/input_xlsx/Flora 002.xlsx
+++ b/input_xlsx/Flora 002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -2465,7 +2465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="118">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -2804,6 +2804,21 @@
   </si>
   <si>
     <t>DESA YENDE, DESA MENARBU, DESA KAYOP</t>
+  </si>
+  <si>
+    <t>Jenis-Jenis Palem di Pulau Roon Kabupaten Teluk Wondama</t>
+  </si>
+  <si>
+    <t>Erce Yemima Sraun</t>
+  </si>
+  <si>
+    <t>Wanggai | Rudi A. Maturbongs</t>
+  </si>
+  <si>
+    <t>UNIPA</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
   </si>
 </sst>
 </file>
@@ -3547,9 +3562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -4588,9 +4603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -4640,6 +4655,30 @@
       </c>
     </row>
     <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2">
+        <v>2006</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" t="s">
+        <v>117</v>
+      </c>
       <c r="J2" s="8"/>
     </row>
   </sheetData>

</xml_diff>